<commit_message>
changes SC and SA for ALLPLAY and MST complete docs for ALLPLAY and MST
</commit_message>
<xml_diff>
--- a/UZ-REPOS/SPA/EDITION/DOC/MST/Модель услуг CT4.xlsx
+++ b/UZ-REPOS/SPA/EDITION/DOC/MST/Модель услуг CT4.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\@MyRepos\FORIS_WORK\UZ-REPOS\SPA\EDITION\DOC\ALLPLAY\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\@MyRepos\FORIS_WORK\UZ-REPOS\SPA\EDITION\DOC\MST\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="32">
   <si>
     <t>Версия</t>
   </si>
@@ -114,28 +114,10 @@
     <t>Абонент зарегистрирован на платформе с услугой ServiceName</t>
   </si>
   <si>
-    <t>FRMOBTV</t>
-  </si>
-  <si>
-    <t>FRMOBTVTEST</t>
-  </si>
-  <si>
-    <t>FRMOBTV1D</t>
-  </si>
-  <si>
-    <t>FRMOBTV7D</t>
-  </si>
-  <si>
-    <t>Мобильное ТВ</t>
-  </si>
-  <si>
-    <t>Мобильное ТВ тест</t>
-  </si>
-  <si>
-    <t>Мобильное ТВ 1 день</t>
-  </si>
-  <si>
-    <t>Мобильное ТВ 7 дней</t>
+    <t>FRCLUBUMS</t>
+  </si>
+  <si>
+    <t>КОНТЕНТ club ums dating</t>
   </si>
 </sst>
 </file>
@@ -146,7 +128,7 @@
     <numFmt numFmtId="164" formatCode="[$-419]General"/>
     <numFmt numFmtId="165" formatCode="#,##0.00&quot; &quot;[$руб.-419];[Red]&quot;-&quot;#,##0.00&quot; &quot;[$руб.-419]"/>
   </numFmts>
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -213,14 +195,6 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="204"/>
-    </font>
-    <font>
-      <b/>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
@@ -237,15 +211,6 @@
     <font>
       <b/>
       <sz val="14"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="204"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -296,7 +261,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="21">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -330,30 +295,6 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
         <color indexed="64"/>
       </left>
       <right style="thin">
@@ -384,19 +325,6 @@
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
         <color indexed="64"/>
       </left>
       <right style="thin">
@@ -439,51 +367,6 @@
       </right>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -498,19 +381,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="medium">
         <color indexed="64"/>
       </left>
@@ -525,21 +395,6 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
         <color indexed="64"/>
       </left>
       <right style="thin">
@@ -552,16 +407,27 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
+      <left style="medium">
+        <color indexed="64"/>
       </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right style="medium">
         <color indexed="64"/>
       </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
+      <top style="medium">
+        <color indexed="64"/>
       </top>
-      <bottom style="thin">
+      <bottom style="medium">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -578,9 +444,9 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="165" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -616,9 +482,6 @@
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -628,67 +491,43 @@
     <xf numFmtId="164" fontId="8" fillId="3" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="6" fillId="4" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="3" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="8" fillId="3" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="4" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="3" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="3" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="5" borderId="3" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="4" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="6" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="4" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="10" fillId="5" borderId="12" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="3" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="3" borderId="15" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="3" borderId="16" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="4" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="3" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="3" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="3" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="3" borderId="18" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="5" borderId="5" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="4" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="5" borderId="12" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="5" borderId="13" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="5" borderId="14" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="5" borderId="8" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="6" borderId="19" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="3" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="10" fillId="5" borderId="13" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1105,7 +944,7 @@
       </c>
     </row>
     <row r="2" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="19" t="s">
+      <c r="A2" s="26" t="s">
         <v>13</v>
       </c>
       <c r="B2" s="9" t="s">
@@ -1116,7 +955,7 @@
       </c>
     </row>
     <row r="3" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="19"/>
+      <c r="A3" s="26"/>
       <c r="B3" s="9" t="s">
         <v>16</v>
       </c>
@@ -1125,7 +964,7 @@
       </c>
     </row>
     <row r="4" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="19" t="s">
+      <c r="A4" s="26" t="s">
         <v>18</v>
       </c>
       <c r="B4" s="9" t="s">
@@ -1136,7 +975,7 @@
       </c>
     </row>
     <row r="5" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="19"/>
+      <c r="A5" s="26"/>
       <c r="B5" s="9" t="s">
         <v>24</v>
       </c>
@@ -1145,7 +984,7 @@
       </c>
     </row>
     <row r="6" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="19"/>
+      <c r="A6" s="26"/>
       <c r="B6" s="9" t="s">
         <v>28</v>
       </c>
@@ -1169,130 +1008,91 @@
   <dimension ref="A1:AMN58"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="13.375" style="15" customWidth="1"/>
-    <col min="2" max="2" width="17.75" style="15" customWidth="1"/>
-    <col min="3" max="3" width="19" style="15" customWidth="1"/>
-    <col min="4" max="4" width="18.5" style="15" customWidth="1"/>
-    <col min="5" max="5" width="17.875" style="15" customWidth="1"/>
-    <col min="6" max="6" width="27.375" style="15" customWidth="1"/>
-    <col min="7" max="7" width="9.875" style="15" customWidth="1"/>
-    <col min="8" max="8" width="28.125" style="15" customWidth="1"/>
-    <col min="9" max="9" width="9.875" style="15" customWidth="1"/>
-    <col min="10" max="10" width="14.125" style="15" customWidth="1"/>
-    <col min="11" max="11" width="13" style="15" customWidth="1"/>
-    <col min="12" max="12" width="11.5" style="15" customWidth="1"/>
-    <col min="13" max="13" width="11.875" style="15" customWidth="1"/>
-    <col min="14" max="14" width="11.5" style="15" customWidth="1"/>
-    <col min="15" max="15" width="18.625" style="15" customWidth="1"/>
-    <col min="16" max="16" width="46.625" style="14" customWidth="1"/>
-    <col min="17" max="1028" width="8.5" style="15" customWidth="1"/>
+    <col min="1" max="1" width="13.375" style="14" customWidth="1"/>
+    <col min="2" max="2" width="17.75" style="14" customWidth="1"/>
+    <col min="3" max="3" width="19" style="14" customWidth="1"/>
+    <col min="4" max="4" width="18.5" style="14" customWidth="1"/>
+    <col min="5" max="5" width="17.875" style="14" customWidth="1"/>
+    <col min="6" max="6" width="27.375" style="14" customWidth="1"/>
+    <col min="7" max="7" width="9.875" style="14" customWidth="1"/>
+    <col min="8" max="8" width="28.125" style="14" customWidth="1"/>
+    <col min="9" max="9" width="9.875" style="14" customWidth="1"/>
+    <col min="10" max="10" width="14.125" style="14" customWidth="1"/>
+    <col min="11" max="11" width="13" style="14" customWidth="1"/>
+    <col min="12" max="12" width="11.5" style="14" customWidth="1"/>
+    <col min="13" max="13" width="11.875" style="14" customWidth="1"/>
+    <col min="14" max="14" width="11.5" style="14" customWidth="1"/>
+    <col min="15" max="15" width="18.625" style="14" customWidth="1"/>
+    <col min="16" max="16" width="46.625" style="13" customWidth="1"/>
+    <col min="17" max="1028" width="8.5" style="14" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" s="4" customFormat="1" ht="85.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="31" t="s">
+      <c r="A1" s="27" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="32"/>
-      <c r="C1" s="32"/>
-      <c r="D1" s="32"/>
-      <c r="E1" s="33"/>
-      <c r="F1" s="20" t="s">
+      <c r="B1" s="28"/>
+      <c r="C1" s="16" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:7" s="4" customFormat="1" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="21" t="s">
+      <c r="A2" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="B2" s="22" t="s">
+      <c r="B2" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="C2" s="23" t="s">
+      <c r="C2" s="19"/>
+    </row>
+    <row r="3" spans="1:7" s="4" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="C3" s="19"/>
+    </row>
+    <row r="4" spans="1:7" s="4" customFormat="1" ht="38.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="B4" s="21" t="s">
         <v>31</v>
       </c>
-      <c r="D2" s="23" t="s">
-        <v>32</v>
-      </c>
-      <c r="E2" s="23" t="s">
-        <v>33</v>
-      </c>
-      <c r="F2" s="24"/>
-    </row>
-    <row r="3" spans="1:7" s="4" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="18" t="s">
-        <v>21</v>
-      </c>
-      <c r="B3" s="16" t="s">
-        <v>30</v>
-      </c>
-      <c r="C3" s="17" t="s">
-        <v>31</v>
-      </c>
-      <c r="D3" s="17" t="s">
-        <v>32</v>
-      </c>
-      <c r="E3" s="13" t="s">
-        <v>33</v>
-      </c>
-      <c r="F3" s="24"/>
-    </row>
-    <row r="4" spans="1:7" s="4" customFormat="1" ht="38.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="25" t="s">
-        <v>22</v>
-      </c>
-      <c r="B4" s="26" t="s">
-        <v>34</v>
-      </c>
-      <c r="C4" s="27" t="s">
-        <v>35</v>
-      </c>
-      <c r="D4" s="28" t="s">
-        <v>36</v>
-      </c>
-      <c r="E4" s="37" t="s">
-        <v>37</v>
-      </c>
-      <c r="F4" s="24"/>
+      <c r="C4" s="19"/>
     </row>
     <row r="5" spans="1:7" s="4" customFormat="1" ht="18.75" x14ac:dyDescent="0.2">
-      <c r="A5" s="36"/>
-      <c r="B5" s="29" t="s">
+      <c r="A5" s="25"/>
+      <c r="B5" s="22" t="s">
         <v>14</v>
       </c>
-      <c r="C5" s="29" t="s">
-        <v>14</v>
-      </c>
-      <c r="D5" s="34" t="s">
-        <v>14</v>
-      </c>
-      <c r="E5" s="34" t="s">
-        <v>14</v>
-      </c>
-      <c r="F5" s="30"/>
+      <c r="C5" s="23"/>
     </row>
     <row r="6" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.2"/>
     <row r="7" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="35"/>
-      <c r="B7" s="35"/>
-      <c r="C7" s="35"/>
-      <c r="D7" s="35"/>
-      <c r="E7" s="35"/>
-      <c r="F7" s="35"/>
-      <c r="G7" s="35"/>
+      <c r="A7" s="24"/>
+      <c r="B7" s="24"/>
+      <c r="C7" s="24"/>
+      <c r="D7" s="24"/>
+      <c r="E7" s="24"/>
+      <c r="F7" s="24"/>
+      <c r="G7" s="24"/>
     </row>
     <row r="8" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="35"/>
-      <c r="B8" s="35"/>
-      <c r="C8" s="35"/>
-      <c r="D8" s="35"/>
-      <c r="E8" s="35"/>
-      <c r="F8" s="35"/>
-      <c r="G8" s="35"/>
+      <c r="A8" s="24"/>
+      <c r="B8" s="24"/>
+      <c r="C8" s="24"/>
+      <c r="D8" s="24"/>
+      <c r="E8" s="24"/>
+      <c r="F8" s="24"/>
+      <c r="G8" s="24"/>
     </row>
     <row r="9" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.2"/>
     <row r="10" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.2"/>
@@ -1321,417 +1121,417 @@
     <row r="33" spans="1:15" s="4" customFormat="1" x14ac:dyDescent="0.2"/>
     <row r="34" spans="1:15" s="4" customFormat="1" x14ac:dyDescent="0.2"/>
     <row r="35" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A35" s="14"/>
-      <c r="B35" s="14"/>
-      <c r="C35" s="14"/>
-      <c r="D35" s="14"/>
-      <c r="E35" s="14"/>
-      <c r="F35" s="14"/>
-      <c r="G35" s="14"/>
-      <c r="H35" s="14"/>
-      <c r="I35" s="14"/>
-      <c r="J35" s="14"/>
-      <c r="K35" s="14"/>
-      <c r="L35" s="14"/>
-      <c r="M35" s="14"/>
-      <c r="N35" s="14"/>
-      <c r="O35" s="14"/>
+      <c r="A35" s="13"/>
+      <c r="B35" s="13"/>
+      <c r="C35" s="13"/>
+      <c r="D35" s="13"/>
+      <c r="E35" s="13"/>
+      <c r="F35" s="13"/>
+      <c r="G35" s="13"/>
+      <c r="H35" s="13"/>
+      <c r="I35" s="13"/>
+      <c r="J35" s="13"/>
+      <c r="K35" s="13"/>
+      <c r="L35" s="13"/>
+      <c r="M35" s="13"/>
+      <c r="N35" s="13"/>
+      <c r="O35" s="13"/>
     </row>
     <row r="36" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A36" s="14"/>
-      <c r="B36" s="14"/>
-      <c r="C36" s="14"/>
-      <c r="D36" s="14"/>
-      <c r="E36" s="14"/>
-      <c r="F36" s="14"/>
-      <c r="G36" s="14"/>
-      <c r="H36" s="14"/>
-      <c r="I36" s="14"/>
-      <c r="J36" s="14"/>
-      <c r="K36" s="14"/>
-      <c r="L36" s="14"/>
-      <c r="M36" s="14"/>
-      <c r="N36" s="14"/>
-      <c r="O36" s="14"/>
+      <c r="A36" s="13"/>
+      <c r="B36" s="13"/>
+      <c r="C36" s="13"/>
+      <c r="D36" s="13"/>
+      <c r="E36" s="13"/>
+      <c r="F36" s="13"/>
+      <c r="G36" s="13"/>
+      <c r="H36" s="13"/>
+      <c r="I36" s="13"/>
+      <c r="J36" s="13"/>
+      <c r="K36" s="13"/>
+      <c r="L36" s="13"/>
+      <c r="M36" s="13"/>
+      <c r="N36" s="13"/>
+      <c r="O36" s="13"/>
     </row>
     <row r="37" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A37" s="14"/>
-      <c r="B37" s="14"/>
-      <c r="C37" s="14"/>
-      <c r="D37" s="14"/>
-      <c r="E37" s="14"/>
-      <c r="F37" s="14"/>
-      <c r="G37" s="14"/>
-      <c r="H37" s="14"/>
-      <c r="I37" s="14"/>
-      <c r="J37" s="14"/>
-      <c r="K37" s="14"/>
-      <c r="L37" s="14"/>
-      <c r="M37" s="14"/>
-      <c r="N37" s="14"/>
-      <c r="O37" s="14"/>
+      <c r="A37" s="13"/>
+      <c r="B37" s="13"/>
+      <c r="C37" s="13"/>
+      <c r="D37" s="13"/>
+      <c r="E37" s="13"/>
+      <c r="F37" s="13"/>
+      <c r="G37" s="13"/>
+      <c r="H37" s="13"/>
+      <c r="I37" s="13"/>
+      <c r="J37" s="13"/>
+      <c r="K37" s="13"/>
+      <c r="L37" s="13"/>
+      <c r="M37" s="13"/>
+      <c r="N37" s="13"/>
+      <c r="O37" s="13"/>
     </row>
     <row r="38" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A38" s="14"/>
-      <c r="B38" s="14"/>
-      <c r="C38" s="14"/>
-      <c r="D38" s="14"/>
-      <c r="E38" s="14"/>
-      <c r="F38" s="14"/>
-      <c r="G38" s="14"/>
-      <c r="H38" s="14"/>
-      <c r="I38" s="14"/>
-      <c r="J38" s="14"/>
-      <c r="K38" s="14"/>
-      <c r="L38" s="14"/>
-      <c r="M38" s="14"/>
-      <c r="N38" s="14"/>
-      <c r="O38" s="14"/>
+      <c r="A38" s="13"/>
+      <c r="B38" s="13"/>
+      <c r="C38" s="13"/>
+      <c r="D38" s="13"/>
+      <c r="E38" s="13"/>
+      <c r="F38" s="13"/>
+      <c r="G38" s="13"/>
+      <c r="H38" s="13"/>
+      <c r="I38" s="13"/>
+      <c r="J38" s="13"/>
+      <c r="K38" s="13"/>
+      <c r="L38" s="13"/>
+      <c r="M38" s="13"/>
+      <c r="N38" s="13"/>
+      <c r="O38" s="13"/>
     </row>
     <row r="39" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A39" s="14"/>
-      <c r="B39" s="14"/>
-      <c r="C39" s="14"/>
-      <c r="D39" s="14"/>
-      <c r="E39" s="14"/>
-      <c r="F39" s="14"/>
-      <c r="G39" s="14"/>
-      <c r="H39" s="14"/>
-      <c r="I39" s="14"/>
-      <c r="J39" s="14"/>
-      <c r="K39" s="14"/>
-      <c r="L39" s="14"/>
-      <c r="M39" s="14"/>
-      <c r="N39" s="14"/>
-      <c r="O39" s="14"/>
+      <c r="A39" s="13"/>
+      <c r="B39" s="13"/>
+      <c r="C39" s="13"/>
+      <c r="D39" s="13"/>
+      <c r="E39" s="13"/>
+      <c r="F39" s="13"/>
+      <c r="G39" s="13"/>
+      <c r="H39" s="13"/>
+      <c r="I39" s="13"/>
+      <c r="J39" s="13"/>
+      <c r="K39" s="13"/>
+      <c r="L39" s="13"/>
+      <c r="M39" s="13"/>
+      <c r="N39" s="13"/>
+      <c r="O39" s="13"/>
     </row>
     <row r="40" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A40" s="14"/>
-      <c r="B40" s="14"/>
-      <c r="C40" s="14"/>
-      <c r="D40" s="14"/>
-      <c r="E40" s="14"/>
-      <c r="F40" s="14"/>
-      <c r="G40" s="14"/>
-      <c r="H40" s="14"/>
-      <c r="I40" s="14"/>
-      <c r="J40" s="14"/>
-      <c r="K40" s="14"/>
-      <c r="L40" s="14"/>
-      <c r="M40" s="14"/>
-      <c r="N40" s="14"/>
-      <c r="O40" s="14"/>
+      <c r="A40" s="13"/>
+      <c r="B40" s="13"/>
+      <c r="C40" s="13"/>
+      <c r="D40" s="13"/>
+      <c r="E40" s="13"/>
+      <c r="F40" s="13"/>
+      <c r="G40" s="13"/>
+      <c r="H40" s="13"/>
+      <c r="I40" s="13"/>
+      <c r="J40" s="13"/>
+      <c r="K40" s="13"/>
+      <c r="L40" s="13"/>
+      <c r="M40" s="13"/>
+      <c r="N40" s="13"/>
+      <c r="O40" s="13"/>
     </row>
     <row r="41" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A41" s="14"/>
-      <c r="B41" s="14"/>
-      <c r="C41" s="14"/>
-      <c r="D41" s="14"/>
-      <c r="E41" s="14"/>
-      <c r="F41" s="14"/>
-      <c r="G41" s="14"/>
-      <c r="H41" s="14"/>
-      <c r="I41" s="14"/>
-      <c r="J41" s="14"/>
-      <c r="K41" s="14"/>
-      <c r="L41" s="14"/>
-      <c r="M41" s="14"/>
-      <c r="N41" s="14"/>
-      <c r="O41" s="14"/>
+      <c r="A41" s="13"/>
+      <c r="B41" s="13"/>
+      <c r="C41" s="13"/>
+      <c r="D41" s="13"/>
+      <c r="E41" s="13"/>
+      <c r="F41" s="13"/>
+      <c r="G41" s="13"/>
+      <c r="H41" s="13"/>
+      <c r="I41" s="13"/>
+      <c r="J41" s="13"/>
+      <c r="K41" s="13"/>
+      <c r="L41" s="13"/>
+      <c r="M41" s="13"/>
+      <c r="N41" s="13"/>
+      <c r="O41" s="13"/>
     </row>
     <row r="42" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A42" s="14"/>
-      <c r="B42" s="14"/>
-      <c r="C42" s="14"/>
-      <c r="D42" s="14"/>
-      <c r="E42" s="14"/>
-      <c r="F42" s="14"/>
-      <c r="G42" s="14"/>
-      <c r="H42" s="14"/>
-      <c r="I42" s="14"/>
-      <c r="J42" s="14"/>
-      <c r="K42" s="14"/>
-      <c r="L42" s="14"/>
-      <c r="M42" s="14"/>
-      <c r="N42" s="14"/>
-      <c r="O42" s="14"/>
+      <c r="A42" s="13"/>
+      <c r="B42" s="13"/>
+      <c r="C42" s="13"/>
+      <c r="D42" s="13"/>
+      <c r="E42" s="13"/>
+      <c r="F42" s="13"/>
+      <c r="G42" s="13"/>
+      <c r="H42" s="13"/>
+      <c r="I42" s="13"/>
+      <c r="J42" s="13"/>
+      <c r="K42" s="13"/>
+      <c r="L42" s="13"/>
+      <c r="M42" s="13"/>
+      <c r="N42" s="13"/>
+      <c r="O42" s="13"/>
     </row>
     <row r="43" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A43" s="14"/>
-      <c r="B43" s="14"/>
-      <c r="C43" s="14"/>
-      <c r="D43" s="14"/>
-      <c r="E43" s="14"/>
-      <c r="F43" s="14"/>
-      <c r="G43" s="14"/>
-      <c r="H43" s="14"/>
-      <c r="I43" s="14"/>
-      <c r="J43" s="14"/>
-      <c r="K43" s="14"/>
-      <c r="L43" s="14"/>
-      <c r="M43" s="14"/>
-      <c r="N43" s="14"/>
-      <c r="O43" s="14"/>
+      <c r="A43" s="13"/>
+      <c r="B43" s="13"/>
+      <c r="C43" s="13"/>
+      <c r="D43" s="13"/>
+      <c r="E43" s="13"/>
+      <c r="F43" s="13"/>
+      <c r="G43" s="13"/>
+      <c r="H43" s="13"/>
+      <c r="I43" s="13"/>
+      <c r="J43" s="13"/>
+      <c r="K43" s="13"/>
+      <c r="L43" s="13"/>
+      <c r="M43" s="13"/>
+      <c r="N43" s="13"/>
+      <c r="O43" s="13"/>
     </row>
     <row r="44" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A44" s="14"/>
-      <c r="B44" s="14"/>
-      <c r="C44" s="14"/>
-      <c r="D44" s="14"/>
-      <c r="E44" s="14"/>
-      <c r="F44" s="14"/>
-      <c r="G44" s="14"/>
-      <c r="H44" s="14"/>
-      <c r="I44" s="14"/>
-      <c r="J44" s="14"/>
-      <c r="K44" s="14"/>
-      <c r="L44" s="14"/>
-      <c r="M44" s="14"/>
-      <c r="N44" s="14"/>
-      <c r="O44" s="14"/>
+      <c r="A44" s="13"/>
+      <c r="B44" s="13"/>
+      <c r="C44" s="13"/>
+      <c r="D44" s="13"/>
+      <c r="E44" s="13"/>
+      <c r="F44" s="13"/>
+      <c r="G44" s="13"/>
+      <c r="H44" s="13"/>
+      <c r="I44" s="13"/>
+      <c r="J44" s="13"/>
+      <c r="K44" s="13"/>
+      <c r="L44" s="13"/>
+      <c r="M44" s="13"/>
+      <c r="N44" s="13"/>
+      <c r="O44" s="13"/>
     </row>
     <row r="45" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A45" s="14"/>
-      <c r="B45" s="14"/>
-      <c r="C45" s="14"/>
-      <c r="D45" s="14"/>
-      <c r="E45" s="14"/>
-      <c r="F45" s="14"/>
-      <c r="G45" s="14"/>
-      <c r="H45" s="14"/>
-      <c r="I45" s="14"/>
-      <c r="J45" s="14"/>
-      <c r="K45" s="14"/>
-      <c r="L45" s="14"/>
-      <c r="M45" s="14"/>
-      <c r="N45" s="14"/>
-      <c r="O45" s="14"/>
+      <c r="A45" s="13"/>
+      <c r="B45" s="13"/>
+      <c r="C45" s="13"/>
+      <c r="D45" s="13"/>
+      <c r="E45" s="13"/>
+      <c r="F45" s="13"/>
+      <c r="G45" s="13"/>
+      <c r="H45" s="13"/>
+      <c r="I45" s="13"/>
+      <c r="J45" s="13"/>
+      <c r="K45" s="13"/>
+      <c r="L45" s="13"/>
+      <c r="M45" s="13"/>
+      <c r="N45" s="13"/>
+      <c r="O45" s="13"/>
     </row>
     <row r="46" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A46" s="14"/>
-      <c r="B46" s="14"/>
-      <c r="C46" s="14"/>
-      <c r="D46" s="14"/>
-      <c r="E46" s="14"/>
-      <c r="F46" s="14"/>
-      <c r="G46" s="14"/>
-      <c r="H46" s="14"/>
-      <c r="I46" s="14"/>
-      <c r="J46" s="14"/>
-      <c r="K46" s="14"/>
-      <c r="L46" s="14"/>
-      <c r="M46" s="14"/>
-      <c r="N46" s="14"/>
-      <c r="O46" s="14"/>
+      <c r="A46" s="13"/>
+      <c r="B46" s="13"/>
+      <c r="C46" s="13"/>
+      <c r="D46" s="13"/>
+      <c r="E46" s="13"/>
+      <c r="F46" s="13"/>
+      <c r="G46" s="13"/>
+      <c r="H46" s="13"/>
+      <c r="I46" s="13"/>
+      <c r="J46" s="13"/>
+      <c r="K46" s="13"/>
+      <c r="L46" s="13"/>
+      <c r="M46" s="13"/>
+      <c r="N46" s="13"/>
+      <c r="O46" s="13"/>
     </row>
     <row r="47" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A47" s="14"/>
-      <c r="B47" s="14"/>
-      <c r="C47" s="14"/>
-      <c r="D47" s="14"/>
-      <c r="E47" s="14"/>
-      <c r="F47" s="14"/>
-      <c r="G47" s="14"/>
-      <c r="H47" s="14"/>
-      <c r="I47" s="14"/>
-      <c r="J47" s="14"/>
-      <c r="K47" s="14"/>
-      <c r="L47" s="14"/>
-      <c r="M47" s="14"/>
-      <c r="N47" s="14"/>
-      <c r="O47" s="14"/>
+      <c r="A47" s="13"/>
+      <c r="B47" s="13"/>
+      <c r="C47" s="13"/>
+      <c r="D47" s="13"/>
+      <c r="E47" s="13"/>
+      <c r="F47" s="13"/>
+      <c r="G47" s="13"/>
+      <c r="H47" s="13"/>
+      <c r="I47" s="13"/>
+      <c r="J47" s="13"/>
+      <c r="K47" s="13"/>
+      <c r="L47" s="13"/>
+      <c r="M47" s="13"/>
+      <c r="N47" s="13"/>
+      <c r="O47" s="13"/>
     </row>
     <row r="48" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A48" s="14"/>
-      <c r="B48" s="14"/>
-      <c r="C48" s="14"/>
-      <c r="D48" s="14"/>
-      <c r="E48" s="14"/>
-      <c r="F48" s="14"/>
-      <c r="G48" s="14"/>
-      <c r="H48" s="14"/>
-      <c r="I48" s="14"/>
-      <c r="J48" s="14"/>
-      <c r="K48" s="14"/>
-      <c r="L48" s="14"/>
-      <c r="M48" s="14"/>
-      <c r="N48" s="14"/>
-      <c r="O48" s="14"/>
+      <c r="A48" s="13"/>
+      <c r="B48" s="13"/>
+      <c r="C48" s="13"/>
+      <c r="D48" s="13"/>
+      <c r="E48" s="13"/>
+      <c r="F48" s="13"/>
+      <c r="G48" s="13"/>
+      <c r="H48" s="13"/>
+      <c r="I48" s="13"/>
+      <c r="J48" s="13"/>
+      <c r="K48" s="13"/>
+      <c r="L48" s="13"/>
+      <c r="M48" s="13"/>
+      <c r="N48" s="13"/>
+      <c r="O48" s="13"/>
     </row>
     <row r="49" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A49" s="14"/>
-      <c r="B49" s="14"/>
-      <c r="C49" s="14"/>
-      <c r="D49" s="14"/>
-      <c r="E49" s="14"/>
-      <c r="F49" s="14"/>
-      <c r="G49" s="14"/>
-      <c r="H49" s="14"/>
-      <c r="I49" s="14"/>
-      <c r="J49" s="14"/>
-      <c r="K49" s="14"/>
-      <c r="L49" s="14"/>
-      <c r="M49" s="14"/>
-      <c r="N49" s="14"/>
-      <c r="O49" s="14"/>
+      <c r="A49" s="13"/>
+      <c r="B49" s="13"/>
+      <c r="C49" s="13"/>
+      <c r="D49" s="13"/>
+      <c r="E49" s="13"/>
+      <c r="F49" s="13"/>
+      <c r="G49" s="13"/>
+      <c r="H49" s="13"/>
+      <c r="I49" s="13"/>
+      <c r="J49" s="13"/>
+      <c r="K49" s="13"/>
+      <c r="L49" s="13"/>
+      <c r="M49" s="13"/>
+      <c r="N49" s="13"/>
+      <c r="O49" s="13"/>
     </row>
     <row r="50" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A50" s="14"/>
-      <c r="B50" s="14"/>
-      <c r="C50" s="14"/>
-      <c r="D50" s="14"/>
-      <c r="E50" s="14"/>
-      <c r="F50" s="14"/>
-      <c r="G50" s="14"/>
-      <c r="H50" s="14"/>
-      <c r="I50" s="14"/>
-      <c r="J50" s="14"/>
-      <c r="K50" s="14"/>
-      <c r="L50" s="14"/>
-      <c r="M50" s="14"/>
-      <c r="N50" s="14"/>
-      <c r="O50" s="14"/>
+      <c r="A50" s="13"/>
+      <c r="B50" s="13"/>
+      <c r="C50" s="13"/>
+      <c r="D50" s="13"/>
+      <c r="E50" s="13"/>
+      <c r="F50" s="13"/>
+      <c r="G50" s="13"/>
+      <c r="H50" s="13"/>
+      <c r="I50" s="13"/>
+      <c r="J50" s="13"/>
+      <c r="K50" s="13"/>
+      <c r="L50" s="13"/>
+      <c r="M50" s="13"/>
+      <c r="N50" s="13"/>
+      <c r="O50" s="13"/>
     </row>
     <row r="51" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A51" s="14"/>
-      <c r="B51" s="14"/>
-      <c r="C51" s="14"/>
-      <c r="D51" s="14"/>
-      <c r="E51" s="14"/>
-      <c r="F51" s="14"/>
-      <c r="G51" s="14"/>
-      <c r="H51" s="14"/>
-      <c r="I51" s="14"/>
-      <c r="J51" s="14"/>
-      <c r="K51" s="14"/>
-      <c r="L51" s="14"/>
-      <c r="M51" s="14"/>
-      <c r="N51" s="14"/>
-      <c r="O51" s="14"/>
+      <c r="A51" s="13"/>
+      <c r="B51" s="13"/>
+      <c r="C51" s="13"/>
+      <c r="D51" s="13"/>
+      <c r="E51" s="13"/>
+      <c r="F51" s="13"/>
+      <c r="G51" s="13"/>
+      <c r="H51" s="13"/>
+      <c r="I51" s="13"/>
+      <c r="J51" s="13"/>
+      <c r="K51" s="13"/>
+      <c r="L51" s="13"/>
+      <c r="M51" s="13"/>
+      <c r="N51" s="13"/>
+      <c r="O51" s="13"/>
     </row>
     <row r="52" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A52" s="14"/>
-      <c r="B52" s="14"/>
-      <c r="C52" s="14"/>
-      <c r="D52" s="14"/>
-      <c r="E52" s="14"/>
-      <c r="F52" s="14"/>
-      <c r="G52" s="14"/>
-      <c r="H52" s="14"/>
-      <c r="I52" s="14"/>
-      <c r="J52" s="14"/>
-      <c r="K52" s="14"/>
-      <c r="L52" s="14"/>
-      <c r="M52" s="14"/>
-      <c r="N52" s="14"/>
-      <c r="O52" s="14"/>
+      <c r="A52" s="13"/>
+      <c r="B52" s="13"/>
+      <c r="C52" s="13"/>
+      <c r="D52" s="13"/>
+      <c r="E52" s="13"/>
+      <c r="F52" s="13"/>
+      <c r="G52" s="13"/>
+      <c r="H52" s="13"/>
+      <c r="I52" s="13"/>
+      <c r="J52" s="13"/>
+      <c r="K52" s="13"/>
+      <c r="L52" s="13"/>
+      <c r="M52" s="13"/>
+      <c r="N52" s="13"/>
+      <c r="O52" s="13"/>
     </row>
     <row r="53" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A53" s="14"/>
-      <c r="B53" s="14"/>
-      <c r="C53" s="14"/>
-      <c r="D53" s="14"/>
-      <c r="E53" s="14"/>
-      <c r="F53" s="14"/>
-      <c r="G53" s="14"/>
-      <c r="H53" s="14"/>
-      <c r="I53" s="14"/>
-      <c r="J53" s="14"/>
-      <c r="K53" s="14"/>
-      <c r="L53" s="14"/>
-      <c r="M53" s="14"/>
-      <c r="N53" s="14"/>
-      <c r="O53" s="14"/>
+      <c r="A53" s="13"/>
+      <c r="B53" s="13"/>
+      <c r="C53" s="13"/>
+      <c r="D53" s="13"/>
+      <c r="E53" s="13"/>
+      <c r="F53" s="13"/>
+      <c r="G53" s="13"/>
+      <c r="H53" s="13"/>
+      <c r="I53" s="13"/>
+      <c r="J53" s="13"/>
+      <c r="K53" s="13"/>
+      <c r="L53" s="13"/>
+      <c r="M53" s="13"/>
+      <c r="N53" s="13"/>
+      <c r="O53" s="13"/>
     </row>
     <row r="54" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A54" s="14"/>
-      <c r="B54" s="14"/>
-      <c r="C54" s="14"/>
-      <c r="D54" s="14"/>
-      <c r="E54" s="14"/>
-      <c r="F54" s="14"/>
-      <c r="G54" s="14"/>
-      <c r="H54" s="14"/>
-      <c r="I54" s="14"/>
-      <c r="J54" s="14"/>
-      <c r="K54" s="14"/>
-      <c r="L54" s="14"/>
-      <c r="M54" s="14"/>
-      <c r="N54" s="14"/>
-      <c r="O54" s="14"/>
+      <c r="A54" s="13"/>
+      <c r="B54" s="13"/>
+      <c r="C54" s="13"/>
+      <c r="D54" s="13"/>
+      <c r="E54" s="13"/>
+      <c r="F54" s="13"/>
+      <c r="G54" s="13"/>
+      <c r="H54" s="13"/>
+      <c r="I54" s="13"/>
+      <c r="J54" s="13"/>
+      <c r="K54" s="13"/>
+      <c r="L54" s="13"/>
+      <c r="M54" s="13"/>
+      <c r="N54" s="13"/>
+      <c r="O54" s="13"/>
     </row>
     <row r="55" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A55" s="14"/>
-      <c r="B55" s="14"/>
-      <c r="C55" s="14"/>
-      <c r="D55" s="14"/>
-      <c r="E55" s="14"/>
-      <c r="F55" s="14"/>
-      <c r="G55" s="14"/>
-      <c r="H55" s="14"/>
-      <c r="I55" s="14"/>
-      <c r="J55" s="14"/>
-      <c r="K55" s="14"/>
-      <c r="L55" s="14"/>
-      <c r="M55" s="14"/>
-      <c r="N55" s="14"/>
-      <c r="O55" s="14"/>
+      <c r="A55" s="13"/>
+      <c r="B55" s="13"/>
+      <c r="C55" s="13"/>
+      <c r="D55" s="13"/>
+      <c r="E55" s="13"/>
+      <c r="F55" s="13"/>
+      <c r="G55" s="13"/>
+      <c r="H55" s="13"/>
+      <c r="I55" s="13"/>
+      <c r="J55" s="13"/>
+      <c r="K55" s="13"/>
+      <c r="L55" s="13"/>
+      <c r="M55" s="13"/>
+      <c r="N55" s="13"/>
+      <c r="O55" s="13"/>
     </row>
     <row r="56" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A56" s="14"/>
-      <c r="B56" s="14"/>
-      <c r="C56" s="14"/>
-      <c r="D56" s="14"/>
-      <c r="E56" s="14"/>
-      <c r="F56" s="14"/>
-      <c r="G56" s="14"/>
-      <c r="H56" s="14"/>
-      <c r="I56" s="14"/>
-      <c r="J56" s="14"/>
-      <c r="K56" s="14"/>
-      <c r="L56" s="14"/>
-      <c r="M56" s="14"/>
-      <c r="N56" s="14"/>
-      <c r="O56" s="14"/>
+      <c r="A56" s="13"/>
+      <c r="B56" s="13"/>
+      <c r="C56" s="13"/>
+      <c r="D56" s="13"/>
+      <c r="E56" s="13"/>
+      <c r="F56" s="13"/>
+      <c r="G56" s="13"/>
+      <c r="H56" s="13"/>
+      <c r="I56" s="13"/>
+      <c r="J56" s="13"/>
+      <c r="K56" s="13"/>
+      <c r="L56" s="13"/>
+      <c r="M56" s="13"/>
+      <c r="N56" s="13"/>
+      <c r="O56" s="13"/>
     </row>
     <row r="57" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A57" s="14"/>
-      <c r="B57" s="14"/>
-      <c r="C57" s="14"/>
-      <c r="D57" s="14"/>
-      <c r="E57" s="14"/>
-      <c r="F57" s="14"/>
-      <c r="G57" s="14"/>
-      <c r="H57" s="14"/>
-      <c r="I57" s="14"/>
-      <c r="J57" s="14"/>
-      <c r="K57" s="14"/>
-      <c r="L57" s="14"/>
-      <c r="M57" s="14"/>
-      <c r="N57" s="14"/>
-      <c r="O57" s="14"/>
+      <c r="A57" s="13"/>
+      <c r="B57" s="13"/>
+      <c r="C57" s="13"/>
+      <c r="D57" s="13"/>
+      <c r="E57" s="13"/>
+      <c r="F57" s="13"/>
+      <c r="G57" s="13"/>
+      <c r="H57" s="13"/>
+      <c r="I57" s="13"/>
+      <c r="J57" s="13"/>
+      <c r="K57" s="13"/>
+      <c r="L57" s="13"/>
+      <c r="M57" s="13"/>
+      <c r="N57" s="13"/>
+      <c r="O57" s="13"/>
     </row>
     <row r="58" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A58" s="14"/>
-      <c r="B58" s="14"/>
-      <c r="C58" s="14"/>
-      <c r="D58" s="14"/>
-      <c r="E58" s="14"/>
-      <c r="F58" s="14"/>
-      <c r="G58" s="14"/>
-      <c r="H58" s="14"/>
-      <c r="I58" s="14"/>
-      <c r="J58" s="14"/>
-      <c r="K58" s="14"/>
-      <c r="L58" s="14"/>
-      <c r="M58" s="14"/>
-      <c r="N58" s="14"/>
-      <c r="O58" s="14"/>
+      <c r="A58" s="13"/>
+      <c r="B58" s="13"/>
+      <c r="C58" s="13"/>
+      <c r="D58" s="13"/>
+      <c r="E58" s="13"/>
+      <c r="F58" s="13"/>
+      <c r="G58" s="13"/>
+      <c r="H58" s="13"/>
+      <c r="I58" s="13"/>
+      <c r="J58" s="13"/>
+      <c r="K58" s="13"/>
+      <c r="L58" s="13"/>
+      <c r="M58" s="13"/>
+      <c r="N58" s="13"/>
+      <c r="O58" s="13"/>
     </row>
   </sheetData>
   <dataConsolidate/>
   <mergeCells count="1">
-    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="A1:B1"/>
   </mergeCells>
   <pageMargins left="0.70000000000000007" right="0.70000000000000007" top="1.1437007874015745" bottom="1.1437007874015745" header="0.74999999999999989" footer="0.74999999999999989"/>
   <pageSetup paperSize="9" fitToWidth="0" fitToHeight="0" orientation="portrait" horizontalDpi="300" r:id="rId1"/>

</xml_diff>